<commit_message>
changes for conf editing
</commit_message>
<xml_diff>
--- a/Default_06_Conferences.xlsx
+++ b/Default_06_Conferences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.boleyn\Documents\GitHub\ncaa-06-scheduler\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5544A810-093A-45ED-805E-513F81553CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA97F96-3939-478F-BDF2-C80BD1EE7ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="2025" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30510" yWindow="1350" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferences" sheetId="2" r:id="rId1"/>
@@ -33868,7 +33868,7 @@
   <dimension ref="A1:AR1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34616,7 +34616,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E14" s="36" t="s">
         <v>7</v>
@@ -34670,7 +34670,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E15" s="36" t="s">
         <v>7</v>

</xml_diff>